<commit_message>
progress on the tedious if else'
</commit_message>
<xml_diff>
--- a/Assignments/Assignment 8/WorldSeriesWinners/Text Files/Sorted Values.xlsx
+++ b/Assignments/Assignment 8/WorldSeriesWinners/Text Files/Sorted Values.xlsx
@@ -462,638 +462,638 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5263B490-15D0-4A74-BA01-9BDD44066D5A}">
-  <dimension ref="A1:C108"/>
+  <dimension ref="A1:B108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="C4">
+      <c r="B4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="C9">
+      <c r="B9">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
-      <c r="C16">
+      <c r="B16">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
-      <c r="C18">
+      <c r="B18">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
-      <c r="C21">
+      <c r="B21">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
-      <c r="C26">
+      <c r="B26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
-      <c r="C28">
+      <c r="B28">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>25</v>
       </c>
-      <c r="C32">
+      <c r="B32">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>21</v>
       </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>16</v>
       </c>
-      <c r="C35">
+      <c r="B35">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>15</v>
       </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>22</v>
       </c>
-      <c r="C41">
+      <c r="B41">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1</v>
       </c>
-      <c r="C43">
+      <c r="B43">
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>18</v>
       </c>
-      <c r="C48">
+      <c r="B48">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>10</v>
       </c>
-      <c r="C50">
+      <c r="B50">
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>19</v>
       </c>
-      <c r="C77">
+      <c r="B77">
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>5</v>
       </c>
-      <c r="C81">
+      <c r="B81">
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>4</v>
       </c>
-      <c r="C88">
+      <c r="B88">
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>28</v>
       </c>
-      <c r="C93">
+      <c r="B93">
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>12</v>
       </c>
-      <c r="C95">
+      <c r="B95">
         <v>11</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>23</v>
       </c>
-      <c r="C106">
+      <c r="B106">
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>11</v>
       </c>
-      <c r="C108">
+      <c r="B108">
         <v>1</v>
       </c>
     </row>

</xml_diff>